<commit_message>
Aggiornamento del file report-checklist.xlsx (20240415.2)
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SINEDXX/Sined_S.r.l./MedWare/24.02.12/report-checklist.xlsx
+++ b/GATEWAY/A1#111SINEDXX/Sined_S.r.l./MedWare/24.02.12/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C0DA03-B360-4CA8-A2E3-5E73B8914A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB4BCDA-6673-4D99-91B7-F2AA78348E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="390" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2403" uniqueCount="970">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2404" uniqueCount="971">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -5006,6 +5006,9 @@
   </si>
   <si>
     <t>subject_application_vendor: Sined_S.r.l.</t>
+  </si>
+  <si>
+    <t>Sined S.r.l.</t>
   </si>
 </sst>
 </file>
@@ -7945,7 +7948,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4:D4"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7990,7 +7993,9 @@
         <v>22</v>
       </c>
       <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
+      <c r="C2" s="46" t="s">
+        <v>970</v>
+      </c>
       <c r="D2" s="45"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -9113,7 +9118,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="37" customFormat="1" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" s="37" customFormat="1" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="35">
         <v>29</v>
       </c>
@@ -9237,7 +9242,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="37" customFormat="1" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" s="37" customFormat="1" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="35">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
SINED : sono stati aggiornati il file data.json ed il file report-checklist.xlsx. Ora, in entrambi, la stringa (appVendor) "Sined_S.r.l." è stata sostituita con la stringa "Sined S.r.l." rendendola congruente con quanto utilizzato nell'omologo campo all'interno del token JWT utilizzato in fase di chiamata al GATEWAY FSE  (20240417.1) .
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SINEDXX/Sined_S.r.l./MedWare/24.02.12/report-checklist.xlsx
+++ b/GATEWAY/A1#111SINEDXX/Sined_S.r.l./MedWare/24.02.12/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my\fse001_ok_20240401.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB4BCDA-6673-4D99-91B7-F2AA78348E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810DBB22-8F1E-4CB6-9CE2-33970FA0FD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="390" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5005,10 +5005,10 @@
     <t>L'applicativo mostra a video l'errore evidenziato nella colonna N. L'operatore, una volta effettuati n-tentativi come suggerito dalla segnalazione di errore, se il problema persiste, contatta l'assistenza tecnica la quale, tramite i log dell'applicativo, identifica e  corregge il problema comunicando, infine, la possibilità di ripetere la validazione</t>
   </si>
   <si>
-    <t>subject_application_vendor: Sined_S.r.l.</t>
-  </si>
-  <si>
     <t>Sined S.r.l.</t>
+  </si>
+  <si>
+    <t>subject_application_vendor: Sined S.r.l.</t>
   </si>
 </sst>
 </file>
@@ -7948,7 +7948,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7994,7 +7994,7 @@
       </c>
       <c r="B2" s="45"/>
       <c r="C2" s="46" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="D2" s="45"/>
       <c r="F2" s="12"/>
@@ -8042,7 +8042,7 @@
       <c r="A4" s="49"/>
       <c r="B4" s="50"/>
       <c r="C4" s="53" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="D4" s="45"/>
       <c r="E4" s="4"/>

</xml_diff>